<commit_message>
modifiche al main per cercare di eliminare tutti i differenti file gen e averne uno solo -> abbandonato
</commit_message>
<xml_diff>
--- a/template_excel/template_SKID_HH.xlsx
+++ b/template_excel/template_SKID_HH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VB2117\CODICE jimmy\complete_test\template_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhoaenergy-my.sharepoint.com/personal/vb2117_nhoa_energy/Documents/Documenti/Jimmy Carradore/jims_code/template_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AE25DD-7504-42E7-9F9B-D6394A942A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{97AE25DD-7504-42E7-9F9B-D6394A942A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EEF21F-CDA1-4CAF-AE05-BEC48CD15C5D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82A76932-9AD5-4175-BD93-A2A70F78D2A2}"/>
+    <workbookView xWindow="-20520" yWindow="-5010" windowWidth="20640" windowHeight="11160" xr2:uid="{82A76932-9AD5-4175-BD93-A2A70F78D2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B7427D-ECF8-421C-ACAA-E30BC134C6AE}">
   <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -9615,7 +9615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Merge dei template excel più aggiornati
</commit_message>
<xml_diff>
--- a/template_excel/template_SKID_HH.xlsx
+++ b/template_excel/template_SKID_HH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VB2117\CODICE jimmy\complete_test\template_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhoaenergy-my.sharepoint.com/personal/vb2117_nhoa_energy/Documents/Documenti/Jimmy Carradore/jims_code/template_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AE25DD-7504-42E7-9F9B-D6394A942A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{97AE25DD-7504-42E7-9F9B-D6394A942A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EEF21F-CDA1-4CAF-AE05-BEC48CD15C5D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82A76932-9AD5-4175-BD93-A2A70F78D2A2}"/>
+    <workbookView xWindow="-20520" yWindow="-5010" windowWidth="20640" windowHeight="11160" xr2:uid="{82A76932-9AD5-4175-BD93-A2A70F78D2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B7427D-ECF8-421C-ACAA-E30BC134C6AE}">
   <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -9615,7 +9615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>91</v>
       </c>

</xml_diff>